<commit_message>
change the tel no and gss section
</commit_message>
<xml_diff>
--- a/export_rfq.xlsx
+++ b/export_rfq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28305" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$52</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <r>
       <t xml:space="preserve">
@@ -35,6 +35,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t/>
     </r>
@@ -46,7 +47,7 @@
     <t>RFQ Number :</t>
   </si>
   <si>
-    <t>2020-138</t>
+    <t>2020-154</t>
   </si>
   <si>
     <t>Mode of Procurement:</t>
@@ -58,7 +59,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>July 17, 2020</t>
+    <t>July 30, 2020</t>
   </si>
   <si>
     <t>Office/End User:</t>
@@ -85,76 +86,16 @@
     <t>PhilGEPS Registration No.:</t>
   </si>
   <si>
-    <t>Please quote your lowest price for the requirements listed hereunder subject to the Terms and Conditions stated below and submit to this office duly signed:</t>
-  </si>
-  <si>
     <t>TERMS AND CONDITIONS:</t>
   </si>
   <si>
-    <t>1. Bidders shall provide correct and accurate information required in this form.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.  The item(s) shall be delivered within 10 calendar days from receipt of Purchase </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Bidders may quote for any or all items. </t>
-  </si>
-  <si>
-    <t>Order (PO).</t>
-  </si>
-  <si>
-    <t>3. Price quotation(s) must be valid for a period of 60 calendar days from the date of submission.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.  The DILG IV-A shall have the right to inspect and/or to test the goods to confirm their </t>
-  </si>
-  <si>
-    <t>4. Price quotation(s) to be denominated in Philippine Peso shall include all taxes duties and/or</t>
-  </si>
-  <si>
-    <t>conformity to the technical specifications.</t>
-  </si>
-  <si>
-    <t>levies payable.</t>
+    <t>7.  Any interlineations, erasures, or overwriting shall be valid only if they are signed or</t>
   </si>
   <si>
     <t>10. Liquidated damages equivalent to one-tenth of one percent (0.1%) of the value of the</t>
   </si>
   <si>
-    <t>5. Quotations exceeding the Approved Budget for the Contract (ABC) shall be rejected.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goods not delivered within the prescribed delivery period shall be imposed per day of delay.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.  Award of contract shall be made to the lowest quotation (for goods) or the highest rated </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The DILG IV-A shall rescind the contract once the cumulative amount of liquidated damages </t>
-  </si>
-  <si>
-    <t xml:space="preserve">offer (for consulting services) which complies with the minimum technical specifiactions and </t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaches ten (10) percent of the amount of the contract, without prejudice to other courses </t>
-  </si>
-  <si>
-    <t>other terms and conditions stated herein.</t>
-  </si>
-  <si>
-    <t>of action and remedies open to it.</t>
-  </si>
-  <si>
-    <t>7.  Any interlineations, erasures, or overwriting shall be valid only if they are signed or</t>
-  </si>
-  <si>
-    <t>initialed by the supplier or its authorized representative(s).</t>
-  </si>
-  <si>
     <t>Approved Budget for the Contract (ABC):</t>
-  </si>
-  <si>
-    <t>PHP 382,302.50</t>
   </si>
   <si>
     <t>DR. CARINA S. CRUZ</t>
@@ -211,66 +152,61 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Customized Washable Face Mask
-Neoprene, Non woven cotton, 2ply lightweight, breathable fabric, Adjustable ear bands, Sublimation design</t>
+    <t>Please quote your lowest price for the requirements listed hereunder subject to the Terms and Conditions stated below and submit to this office duly signed:</t>
   </si>
   <si>
-    <t>piece</t>
+    <t>1. Bidders shall provide correct and accurate information required in this form.</t>
   </si>
   <si>
-    <t>Alcohol 70%, (1 Gal)
-qwe</t>
+    <t xml:space="preserve">2. Bidders may quote for any or all items. </t>
   </si>
   <si>
-    <t>gallon</t>
+    <t>3. Price quotation(s) must be valid for a period of 60 calendar days from the date of submission.</t>
   </si>
   <si>
-    <t>Absorbent gauze 36sX100yds-2ply 40X28x24mesh
-qwe</t>
+    <t>4. Price quotation(s) to be denominated in Philippine Peso shall include all taxes duties and/or</t>
   </si>
   <si>
-    <t>pack</t>
+    <t>5. Quotations exceeding the Approved Budget for the Contract (ABC) shall be rejected.</t>
   </si>
   <si>
-    <t>1,552.50</t>
+    <t xml:space="preserve">6.  Award of contract shall be made to the lowest quotation (for goods) or the highest rated </t>
   </si>
   <si>
-    <t>Warranty:</t>
+    <t xml:space="preserve">offer (for consulting services) which complies with the minimum technical specifiactions and </t>
   </si>
   <si>
-    <t>Price Validity:</t>
+    <t>levies payable.</t>
   </si>
   <si>
-    <t>TOTAL</t>
+    <t>other terms and conditions stated herein.</t>
   </si>
   <si>
-    <t>SUPPLIER DETAILS</t>
+    <t>initialed by the supplier or its authorized representative(s).</t>
   </si>
   <si>
-    <t>After having carefully read and accepted your General Conditions, I / WE quote on the item(s) at prices noted above.</t>
+    <t>Order (PO).</t>
   </si>
   <si>
-    <t>Name:</t>
+    <t>conformity to the technical specifications.</t>
   </si>
   <si>
-    <t>Contact:</t>
+    <t xml:space="preserve">goods not delivered within the prescribed delivery period shall be imposed per day of delay.  </t>
   </si>
   <si>
-    <t>Signature</t>
+    <t xml:space="preserve">reaches ten (10) percent of the amount of the contract, without prejudice to other courses </t>
   </si>
   <si>
-    <t>NOTE:
-*In order to be eligible for this procurement, suppliers/service providers must submit together with the quotation the following Eligibility Documents:
-   1. Valid Business Permit 2021 ( Application for renewal with Official Receipt 2021)
-   2. PhilGEPS Registration No. (Please indicate on the space provided above)
-   3. a. Any documents to prove that the signatory of the quotation is autorized representative of the company.
-       b. Photocopy of ID bearing the pictures/ signature of the representatives.
-   4. Accomplished and Notarized Omnibus Sworn Statement
- * Please submit your quotation using our official Request for Quotation (RFQ) Form. You can secure a copy of the 
-RFQ from the General Services and Supply Section, Finance and Administrative Division. 
- *Please submit your quotation together with the Eligibility Documents through any of the following : 
-       a. Email us at dilg4a.bac@gmail.com
-     b. Deliver on hand at the receiving area of DILG IV-A CALABARZON, Andenson Bldg1. National Highway, Parian, Calamba City, Laguna</t>
+    <t>of action and remedies open to it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.  The DILG IV-A shall have the right to inspect and/or to test the goods to confirm their </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.  The item(s) shall be delivered within 10 calendar days from receipt of Purchase </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The DILG IV-A shall rescind the contract once the cumulative amount of liquidated damages </t>
   </si>
 </sst>
 </file>
@@ -282,7 +218,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00;[Red]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -293,63 +229,102 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -357,49 +332,23 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <b/>
+      <i/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,14 +370,8 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB5B8BC"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -505,6 +448,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -553,19 +516,12 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -594,14 +550,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -609,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -655,19 +613,19 @@
     <xf numFmtId="15" fontId="1" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -688,17 +646,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -710,34 +668,34 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -756,147 +714,117 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -905,19 +833,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -926,113 +854,32 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1056,9 +903,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>116205</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>127635</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="752475" cy="762000"/>
     <xdr:pic>
@@ -1076,8 +923,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
+          <a:off x="116205" y="135255"/>
+          <a:ext cx="752475" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1152,6 +999,91 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>453957</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>48639</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>166181</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>77011</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="834957" y="705256"/>
+          <a:ext cx="2638628" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>(02)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> 8876-3456 loc. 7403</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="900">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1198,7 +1130,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1233,7 +1165,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1447,8 +1379,8 @@
   </sheetPr>
   <dimension ref="A1:L844"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A46" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A32" zoomScale="160" zoomScaleNormal="55" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,11 +1517,11 @@
       <c r="I11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="91" t="s">
+      <c r="J11" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="92"/>
-      <c r="L11" s="93"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="83"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
@@ -1597,21 +1529,21 @@
         <v>4</v>
       </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="94" t="s">
+      <c r="D12" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="94"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="94"/>
-      <c r="H12" s="95"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="85"/>
       <c r="I12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="96" t="s">
+      <c r="J12" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="97"/>
-      <c r="L12" s="98"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="88"/>
     </row>
     <row r="13" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
@@ -1628,62 +1560,62 @@
       <c r="L13" s="17"/>
     </row>
     <row r="14" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="106" t="s">
+      <c r="A14" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="106"/>
-      <c r="C14" s="91" t="s">
+      <c r="B14" s="96"/>
+      <c r="C14" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="93"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="83"/>
     </row>
     <row r="15" spans="1:12" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="106" t="s">
+      <c r="A15" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="106"/>
-      <c r="C15" s="107" t="s">
+      <c r="B15" s="96"/>
+      <c r="C15" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="108"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="108"/>
-      <c r="K15" s="108"/>
-      <c r="L15" s="109"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="99"/>
     </row>
     <row r="16" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="106" t="s">
+      <c r="A16" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="106"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="93"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="82"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="82"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="83"/>
     </row>
     <row r="17" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="106" t="s">
+      <c r="A17" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="106"/>
+      <c r="B17" s="96"/>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
@@ -1696,10 +1628,10 @@
       <c r="L17" s="28"/>
     </row>
     <row r="18" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="106" t="s">
+      <c r="A18" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="106"/>
+      <c r="B18" s="96"/>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
       <c r="E18" s="27"/>
@@ -1712,10 +1644,10 @@
       <c r="L18" s="28"/>
     </row>
     <row r="19" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="105" t="s">
+      <c r="A19" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="105"/>
+      <c r="B19" s="95"/>
       <c r="C19" s="73"/>
       <c r="D19" s="73"/>
       <c r="E19" s="73"/>
@@ -1729,7 +1661,7 @@
     </row>
     <row r="20" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="75" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B20" s="76"/>
       <c r="C20" s="76"/>
@@ -1744,24 +1676,24 @@
       <c r="L20" s="77"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="102" t="s">
-        <v>17</v>
+      <c r="A21" s="92" t="s">
+        <v>16</v>
       </c>
-      <c r="B21" s="102"/>
-      <c r="C21" s="102"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="102"/>
-      <c r="I21" s="102"/>
-      <c r="J21" s="102"/>
-      <c r="K21" s="102"/>
-      <c r="L21" s="102"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="92"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="92"/>
+      <c r="I21" s="92"/>
+      <c r="J21" s="92"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="92"/>
     </row>
     <row r="22" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="67" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -1769,7 +1701,7 @@
       <c r="E22" s="41"/>
       <c r="F22" s="42"/>
       <c r="G22" s="72" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="20"/>
@@ -1779,7 +1711,7 @@
     </row>
     <row r="23" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="66" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
@@ -1787,7 +1719,7 @@
       <c r="E23" s="45"/>
       <c r="F23" s="46"/>
       <c r="G23" s="70" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H23" s="23"/>
       <c r="I23" s="24"/>
@@ -1797,7 +1729,7 @@
     </row>
     <row r="24" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="66" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
@@ -1805,7 +1737,7 @@
       <c r="E24" s="45"/>
       <c r="F24" s="46"/>
       <c r="G24" s="69" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="H24" s="23"/>
       <c r="I24" s="24"/>
@@ -1815,7 +1747,7 @@
     </row>
     <row r="25" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="66" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
@@ -1823,7 +1755,7 @@
       <c r="E25" s="45"/>
       <c r="F25" s="46"/>
       <c r="G25" s="69" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="H25" s="48"/>
       <c r="I25" s="49"/>
@@ -1833,7 +1765,7 @@
     </row>
     <row r="26" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="66" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
@@ -1841,7 +1773,7 @@
       <c r="E26" s="45"/>
       <c r="F26" s="46"/>
       <c r="G26" s="26" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H26" s="23"/>
       <c r="I26" s="24"/>
@@ -1851,7 +1783,7 @@
     </row>
     <row r="27" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="66" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -1859,7 +1791,7 @@
       <c r="E27" s="45"/>
       <c r="F27" s="46"/>
       <c r="G27" s="71" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="H27" s="23"/>
       <c r="I27" s="24"/>
@@ -1869,7 +1801,7 @@
     </row>
     <row r="28" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="66" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -1877,7 +1809,7 @@
       <c r="E28" s="45"/>
       <c r="F28" s="46"/>
       <c r="G28" s="71" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="H28" s="23"/>
       <c r="I28" s="24"/>
@@ -1887,7 +1819,7 @@
     </row>
     <row r="29" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="66" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
@@ -1895,7 +1827,7 @@
       <c r="E29" s="45"/>
       <c r="F29" s="46"/>
       <c r="G29" s="71" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H29" s="23"/>
       <c r="I29" s="24"/>
@@ -1905,7 +1837,7 @@
     </row>
     <row r="30" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="66" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
@@ -1913,7 +1845,7 @@
       <c r="E30" s="45"/>
       <c r="F30" s="46"/>
       <c r="G30" s="71" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="H30" s="23"/>
       <c r="I30" s="24"/>
@@ -1923,7 +1855,7 @@
     </row>
     <row r="31" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="68" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
@@ -1939,7 +1871,7 @@
     </row>
     <row r="32" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="68" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -1954,16 +1886,16 @@
       <c r="L32" s="46"/>
     </row>
     <row r="33" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="103" t="s">
-        <v>38</v>
+      <c r="A33" s="93" t="s">
+        <v>19</v>
       </c>
-      <c r="B33" s="103"/>
-      <c r="C33" s="104" t="s">
-        <v>39</v>
+      <c r="B33" s="93"/>
+      <c r="C33" s="94">
+        <v>158400</v>
       </c>
-      <c r="D33" s="104"/>
-      <c r="E33" s="104"/>
-      <c r="F33" s="104"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
       <c r="G33" s="50"/>
       <c r="H33" s="50"/>
       <c r="I33" s="51"/>
@@ -1972,12 +1904,12 @@
       <c r="L33" s="52"/>
     </row>
     <row r="34" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="103"/>
-      <c r="B34" s="103"/>
-      <c r="C34" s="104"/>
-      <c r="D34" s="104"/>
-      <c r="E34" s="104"/>
-      <c r="F34" s="104"/>
+      <c r="A34" s="93"/>
+      <c r="B34" s="93"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="94"/>
+      <c r="F34" s="94"/>
       <c r="G34" s="53"/>
       <c r="H34" s="53"/>
       <c r="I34" s="30"/>
@@ -1986,368 +1918,318 @@
       <c r="L34" s="54"/>
     </row>
     <row r="35" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="103"/>
-      <c r="B35" s="103"/>
-      <c r="C35" s="104"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="104"/>
+      <c r="A35" s="93"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
       <c r="G35" s="55"/>
       <c r="H35" s="55"/>
       <c r="I35" s="14" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
       <c r="L35" s="54"/>
     </row>
     <row r="36" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="103"/>
-      <c r="B36" s="103"/>
-      <c r="C36" s="104"/>
-      <c r="D36" s="104"/>
-      <c r="E36" s="104"/>
-      <c r="F36" s="104"/>
+      <c r="A36" s="93"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="94"/>
       <c r="G36" s="56"/>
-      <c r="H36" s="110" t="s">
-        <v>41</v>
+      <c r="H36" s="100" t="s">
+        <v>21</v>
       </c>
-      <c r="I36" s="110"/>
-      <c r="J36" s="110"/>
-      <c r="K36" s="110"/>
+      <c r="I36" s="100"/>
+      <c r="J36" s="100"/>
+      <c r="K36" s="100"/>
       <c r="L36" s="57"/>
     </row>
     <row r="37" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="99"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="100"/>
-      <c r="F37" s="100"/>
-      <c r="G37" s="100"/>
-      <c r="H37" s="100"/>
-      <c r="I37" s="100"/>
-      <c r="J37" s="100"/>
-      <c r="K37" s="100"/>
-      <c r="L37" s="101"/>
+      <c r="A37" s="89"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="90"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="90"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="90"/>
+      <c r="H37" s="90"/>
+      <c r="I37" s="90"/>
+      <c r="J37" s="90"/>
+      <c r="K37" s="90"/>
+      <c r="L37" s="91"/>
     </row>
     <row r="38" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="103" t="s">
-        <v>42</v>
+      <c r="A38" s="93" t="s">
+        <v>22</v>
       </c>
-      <c r="B38" s="112" t="s">
-        <v>43</v>
+      <c r="B38" s="102" t="s">
+        <v>23</v>
       </c>
-      <c r="C38" s="111" t="s">
-        <v>44</v>
+      <c r="C38" s="101" t="s">
+        <v>24</v>
       </c>
-      <c r="D38" s="103" t="s">
-        <v>45</v>
+      <c r="D38" s="93" t="s">
+        <v>25</v>
       </c>
-      <c r="E38" s="120" t="s">
-        <v>46</v>
+      <c r="E38" s="110" t="s">
+        <v>26</v>
       </c>
-      <c r="F38" s="118" t="s">
-        <v>47</v>
+      <c r="F38" s="108" t="s">
+        <v>27</v>
       </c>
-      <c r="G38" s="118"/>
-      <c r="H38" s="118"/>
-      <c r="I38" s="118"/>
-      <c r="J38" s="118"/>
-      <c r="K38" s="118"/>
-      <c r="L38" s="119"/>
+      <c r="G38" s="108"/>
+      <c r="H38" s="108"/>
+      <c r="I38" s="108"/>
+      <c r="J38" s="108"/>
+      <c r="K38" s="108"/>
+      <c r="L38" s="109"/>
     </row>
     <row r="39" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="103"/>
-      <c r="B39" s="113"/>
-      <c r="C39" s="111"/>
-      <c r="D39" s="103"/>
-      <c r="E39" s="120"/>
-      <c r="F39" s="116" t="s">
-        <v>48</v>
+      <c r="A39" s="93"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="101"/>
+      <c r="D39" s="93"/>
+      <c r="E39" s="110"/>
+      <c r="F39" s="106" t="s">
+        <v>28</v>
       </c>
-      <c r="G39" s="117"/>
-      <c r="H39" s="117"/>
-      <c r="I39" s="115" t="s">
-        <v>49</v>
+      <c r="G39" s="107"/>
+      <c r="H39" s="107"/>
+      <c r="I39" s="105" t="s">
+        <v>29</v>
       </c>
-      <c r="J39" s="115"/>
-      <c r="K39" s="121" t="s">
-        <v>50</v>
+      <c r="J39" s="105"/>
+      <c r="K39" s="111" t="s">
+        <v>30</v>
       </c>
-      <c r="L39" s="122"/>
+      <c r="L39" s="112"/>
     </row>
     <row r="40" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="103"/>
-      <c r="B40" s="113"/>
-      <c r="C40" s="111"/>
-      <c r="D40" s="103"/>
-      <c r="E40" s="120"/>
-      <c r="F40" s="116"/>
-      <c r="G40" s="117"/>
-      <c r="H40" s="117"/>
-      <c r="I40" s="115"/>
-      <c r="J40" s="115"/>
-      <c r="K40" s="123"/>
-      <c r="L40" s="124"/>
+      <c r="A40" s="93"/>
+      <c r="B40" s="103"/>
+      <c r="C40" s="101"/>
+      <c r="D40" s="93"/>
+      <c r="E40" s="110"/>
+      <c r="F40" s="106"/>
+      <c r="G40" s="107"/>
+      <c r="H40" s="107"/>
+      <c r="I40" s="105"/>
+      <c r="J40" s="105"/>
+      <c r="K40" s="113"/>
+      <c r="L40" s="114"/>
     </row>
     <row r="41" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="103"/>
-      <c r="B41" s="113"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="103"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="116"/>
-      <c r="G41" s="117"/>
-      <c r="H41" s="117"/>
-      <c r="I41" s="115"/>
-      <c r="J41" s="115"/>
-      <c r="K41" s="123"/>
-      <c r="L41" s="124"/>
+      <c r="A41" s="93"/>
+      <c r="B41" s="103"/>
+      <c r="C41" s="101"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="106"/>
+      <c r="G41" s="107"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="105"/>
+      <c r="J41" s="105"/>
+      <c r="K41" s="113"/>
+      <c r="L41" s="114"/>
     </row>
     <row r="42" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="103"/>
-      <c r="B42" s="113"/>
-      <c r="C42" s="111"/>
-      <c r="D42" s="103"/>
-      <c r="E42" s="120"/>
-      <c r="F42" s="116"/>
-      <c r="G42" s="117"/>
-      <c r="H42" s="117"/>
-      <c r="I42" s="115"/>
-      <c r="J42" s="115"/>
-      <c r="K42" s="123"/>
-      <c r="L42" s="124"/>
+      <c r="A42" s="93"/>
+      <c r="B42" s="103"/>
+      <c r="C42" s="101"/>
+      <c r="D42" s="93"/>
+      <c r="E42" s="110"/>
+      <c r="F42" s="106"/>
+      <c r="G42" s="107"/>
+      <c r="H42" s="107"/>
+      <c r="I42" s="105"/>
+      <c r="J42" s="105"/>
+      <c r="K42" s="113"/>
+      <c r="L42" s="114"/>
     </row>
     <row r="43" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="103"/>
-      <c r="B43" s="113"/>
-      <c r="C43" s="111"/>
-      <c r="D43" s="103"/>
-      <c r="E43" s="120"/>
-      <c r="F43" s="127" t="s">
-        <v>51</v>
+      <c r="A43" s="93"/>
+      <c r="B43" s="103"/>
+      <c r="C43" s="101"/>
+      <c r="D43" s="93"/>
+      <c r="E43" s="110"/>
+      <c r="F43" s="117" t="s">
+        <v>31</v>
       </c>
-      <c r="G43" s="129" t="s">
-        <v>52</v>
+      <c r="G43" s="119" t="s">
+        <v>32</v>
       </c>
-      <c r="H43" s="131" t="s">
-        <v>53</v>
+      <c r="H43" s="121" t="s">
+        <v>33</v>
       </c>
-      <c r="I43" s="133" t="s">
-        <v>54</v>
+      <c r="I43" s="123" t="s">
+        <v>34</v>
       </c>
-      <c r="J43" s="134" t="s">
-        <v>55</v>
+      <c r="J43" s="124" t="s">
+        <v>35</v>
       </c>
-      <c r="K43" s="123"/>
-      <c r="L43" s="124"/>
+      <c r="K43" s="113"/>
+      <c r="L43" s="114"/>
     </row>
     <row r="44" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="103"/>
-      <c r="B44" s="114"/>
-      <c r="C44" s="111"/>
-      <c r="D44" s="103"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="128"/>
-      <c r="G44" s="130"/>
-      <c r="H44" s="132"/>
-      <c r="I44" s="134"/>
-      <c r="J44" s="117"/>
-      <c r="K44" s="125"/>
-      <c r="L44" s="126"/>
-    </row>
-    <row r="45" spans="1:12" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="81">
-        <v>1</v>
-      </c>
-      <c r="B45" s="81" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="82">
-        <v>2000</v>
-      </c>
-      <c r="D45" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="E45" s="84">
-        <v>190</v>
-      </c>
-      <c r="F45" s="85"/>
-      <c r="G45" s="86"/>
-      <c r="H45" s="86"/>
-      <c r="I45" s="85"/>
-      <c r="J45" s="85"/>
-      <c r="K45" s="85"/>
-      <c r="L45" s="85"/>
-    </row>
-    <row r="46" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="81">
-        <v>2</v>
-      </c>
-      <c r="B46" s="81" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="82">
-        <v>1</v>
-      </c>
-      <c r="D46" s="83" t="s">
-        <v>59</v>
-      </c>
-      <c r="E46" s="84">
-        <v>750</v>
-      </c>
-      <c r="F46" s="85"/>
-      <c r="G46" s="86"/>
-      <c r="H46" s="86"/>
-      <c r="I46" s="85"/>
-      <c r="J46" s="85"/>
-      <c r="K46" s="85"/>
-      <c r="L46" s="85"/>
-    </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="81">
-        <v>3</v>
-      </c>
-      <c r="B47" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" s="82">
-        <v>1</v>
-      </c>
-      <c r="D47" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="E47" s="84" t="s">
-        <v>62</v>
-      </c>
-      <c r="F47" s="87"/>
-      <c r="G47" s="88"/>
-      <c r="H47" s="88"/>
-      <c r="I47" s="87"/>
-      <c r="J47" s="87"/>
-      <c r="K47" s="87"/>
-      <c r="L47" s="87"/>
-    </row>
-    <row r="48" spans="1:12" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="135" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="136"/>
-      <c r="C48" s="136"/>
-      <c r="D48" s="137"/>
-      <c r="E48" s="138"/>
-      <c r="F48" s="136"/>
-      <c r="G48" s="138"/>
-      <c r="H48" s="138"/>
-      <c r="I48" s="136"/>
-      <c r="J48" s="136"/>
-      <c r="K48" s="136"/>
-      <c r="L48" s="139"/>
-    </row>
-    <row r="49" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="89" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" s="90"/>
-      <c r="C49" s="145"/>
-      <c r="D49" s="146"/>
-      <c r="E49" s="147"/>
-      <c r="F49" s="140" t="s">
-        <v>64</v>
-      </c>
-      <c r="G49" s="141"/>
-      <c r="H49" s="142"/>
-      <c r="I49" s="143"/>
-      <c r="J49" s="89" t="s">
-        <v>65</v>
-      </c>
-      <c r="K49" s="144"/>
-      <c r="L49" s="143"/>
-    </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="148" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="149"/>
-      <c r="C50" s="149"/>
-      <c r="D50" s="150"/>
-      <c r="E50" s="151"/>
-      <c r="F50" s="149"/>
-      <c r="G50" s="151"/>
-      <c r="H50" s="151"/>
-      <c r="I50" s="149"/>
-      <c r="J50" s="149"/>
-      <c r="K50" s="149"/>
-      <c r="L50" s="152"/>
-    </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="153" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="154"/>
-      <c r="C51" s="154"/>
-      <c r="D51" s="155"/>
-      <c r="E51" s="156"/>
-      <c r="F51" s="154"/>
-      <c r="G51" s="156"/>
-      <c r="H51" s="156"/>
-      <c r="I51" s="154"/>
-      <c r="J51" s="154"/>
-      <c r="K51" s="154"/>
-      <c r="L51" s="157"/>
-    </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="143"/>
-      <c r="C52" s="158"/>
-      <c r="D52" s="146"/>
-      <c r="E52" s="159"/>
-      <c r="F52" s="160"/>
-      <c r="G52" s="159"/>
-      <c r="H52" s="159"/>
-      <c r="I52" s="160"/>
-      <c r="J52" s="160"/>
-      <c r="K52" s="160"/>
-      <c r="L52" s="143"/>
-    </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="140" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53" s="143"/>
-      <c r="C53" s="158"/>
-      <c r="D53" s="146"/>
-      <c r="E53" s="159"/>
-      <c r="F53" s="160"/>
-      <c r="G53" s="159"/>
-      <c r="H53" s="159"/>
-      <c r="I53" s="160"/>
-      <c r="J53" s="160"/>
-      <c r="K53" s="160"/>
-      <c r="L53" s="143"/>
-    </row>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="140" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" s="143"/>
-      <c r="C54" s="158"/>
-      <c r="D54" s="146"/>
-      <c r="E54" s="159"/>
-      <c r="F54" s="143"/>
-      <c r="G54" s="161" t="s">
-        <v>6</v>
-      </c>
-      <c r="H54" s="147"/>
-      <c r="I54" s="158"/>
-      <c r="J54" s="160"/>
-      <c r="K54" s="160"/>
-      <c r="L54" s="143"/>
-    </row>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="93"/>
+      <c r="B44" s="104"/>
+      <c r="C44" s="101"/>
+      <c r="D44" s="93"/>
+      <c r="E44" s="110"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="120"/>
+      <c r="H44" s="122"/>
+      <c r="I44" s="124"/>
+      <c r="J44" s="107"/>
+      <c r="K44" s="115"/>
+      <c r="L44" s="116"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="58"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="58"/>
+      <c r="K45" s="58"/>
+      <c r="L45" s="58"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="78"/>
+      <c r="B47" s="78"/>
+      <c r="C47" s="78"/>
+      <c r="D47" s="79"/>
+      <c r="E47" s="80"/>
+      <c r="F47" s="78"/>
+      <c r="G47" s="80"/>
+      <c r="H47" s="80"/>
+      <c r="I47" s="78"/>
+      <c r="J47" s="78"/>
+      <c r="K47" s="78"/>
+      <c r="L47" s="78"/>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="78"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="79"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="80"/>
+      <c r="H48" s="80"/>
+      <c r="I48" s="78"/>
+      <c r="J48" s="78"/>
+      <c r="K48" s="78"/>
+      <c r="L48" s="78"/>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="78"/>
+      <c r="B49" s="78"/>
+      <c r="C49" s="78"/>
+      <c r="D49" s="79"/>
+      <c r="E49" s="80"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="80"/>
+      <c r="H49" s="80"/>
+      <c r="I49" s="78"/>
+      <c r="J49" s="78"/>
+      <c r="K49" s="78"/>
+      <c r="L49" s="78"/>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="78"/>
+      <c r="B50" s="78"/>
+      <c r="C50" s="78"/>
+      <c r="D50" s="79"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="78"/>
+      <c r="G50" s="80"/>
+      <c r="H50" s="80"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
+      <c r="L50" s="78"/>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="78"/>
+      <c r="B51" s="78"/>
+      <c r="C51" s="78"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="80"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="80"/>
+      <c r="H51" s="80"/>
+      <c r="I51" s="78"/>
+      <c r="J51" s="78"/>
+      <c r="K51" s="78"/>
+      <c r="L51" s="78"/>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="78"/>
+      <c r="B52" s="78"/>
+      <c r="C52" s="78"/>
+      <c r="D52" s="79"/>
+      <c r="E52" s="80"/>
+      <c r="F52" s="78"/>
+      <c r="G52" s="80"/>
+      <c r="H52" s="80"/>
+      <c r="I52" s="78"/>
+      <c r="J52" s="78"/>
+      <c r="K52" s="78"/>
+      <c r="L52" s="78"/>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="78"/>
+      <c r="B53" s="78"/>
+      <c r="C53" s="78"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="80"/>
+      <c r="F53" s="78"/>
+      <c r="G53" s="80"/>
+      <c r="H53" s="80"/>
+      <c r="I53" s="78"/>
+      <c r="J53" s="78"/>
+      <c r="K53" s="78"/>
+      <c r="L53" s="78"/>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="78"/>
+      <c r="B54" s="78"/>
+      <c r="C54" s="78"/>
+      <c r="D54" s="79"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="78"/>
+      <c r="G54" s="80"/>
+      <c r="H54" s="80"/>
+      <c r="I54" s="78"/>
+      <c r="J54" s="78"/>
+      <c r="K54" s="78"/>
+      <c r="L54" s="78"/>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="78"/>
       <c r="B55" s="78"/>
       <c r="C55" s="78"/>
@@ -2361,7 +2243,7 @@
       <c r="K55" s="78"/>
       <c r="L55" s="78"/>
     </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="78"/>
       <c r="B56" s="78"/>
       <c r="C56" s="78"/>
@@ -2375,7 +2257,7 @@
       <c r="K56" s="78"/>
       <c r="L56" s="78"/>
     </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="78"/>
       <c r="B57" s="78"/>
       <c r="C57" s="78"/>
@@ -2389,7 +2271,7 @@
       <c r="K57" s="78"/>
       <c r="L57" s="78"/>
     </row>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="78"/>
       <c r="B58" s="78"/>
       <c r="C58" s="78"/>
@@ -2403,7 +2285,7 @@
       <c r="K58" s="78"/>
       <c r="L58" s="78"/>
     </row>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="78"/>
       <c r="B59" s="78"/>
       <c r="C59" s="78"/>
@@ -2417,7 +2299,7 @@
       <c r="K59" s="78"/>
       <c r="L59" s="78"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="78"/>
       <c r="B60" s="78"/>
       <c r="C60" s="78"/>
@@ -2431,7 +2313,7 @@
       <c r="K60" s="78"/>
       <c r="L60" s="78"/>
     </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="78"/>
       <c r="B61" s="78"/>
       <c r="C61" s="78"/>
@@ -2445,7 +2327,7 @@
       <c r="K61" s="78"/>
       <c r="L61" s="78"/>
     </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="78"/>
       <c r="B62" s="78"/>
       <c r="C62" s="78"/>
@@ -2459,7 +2341,7 @@
       <c r="K62" s="78"/>
       <c r="L62" s="78"/>
     </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="78"/>
       <c r="B63" s="78"/>
       <c r="C63" s="78"/>
@@ -2473,7 +2355,7 @@
       <c r="K63" s="78"/>
       <c r="L63" s="78"/>
     </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="78"/>
       <c r="B64" s="78"/>
       <c r="C64" s="78"/>
@@ -2487,7 +2369,7 @@
       <c r="K64" s="78"/>
       <c r="L64" s="78"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="78"/>
       <c r="B65" s="78"/>
       <c r="C65" s="78"/>
@@ -2501,7 +2383,7 @@
       <c r="K65" s="78"/>
       <c r="L65" s="78"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="78"/>
       <c r="B66" s="78"/>
       <c r="C66" s="78"/>
@@ -2515,7 +2397,7 @@
       <c r="K66" s="78"/>
       <c r="L66" s="78"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="78"/>
       <c r="B67" s="78"/>
       <c r="C67" s="78"/>
@@ -2529,7 +2411,7 @@
       <c r="K67" s="78"/>
       <c r="L67" s="78"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="78"/>
       <c r="B68" s="78"/>
       <c r="C68" s="78"/>
@@ -2543,7 +2425,7 @@
       <c r="K68" s="78"/>
       <c r="L68" s="78"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="78"/>
       <c r="B69" s="78"/>
       <c r="C69" s="78"/>
@@ -2557,7 +2439,7 @@
       <c r="K69" s="78"/>
       <c r="L69" s="78"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="78"/>
       <c r="B70" s="78"/>
       <c r="C70" s="78"/>
@@ -2571,7 +2453,7 @@
       <c r="K70" s="78"/>
       <c r="L70" s="78"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="78"/>
       <c r="B71" s="78"/>
       <c r="C71" s="78"/>
@@ -2585,7 +2467,7 @@
       <c r="K71" s="78"/>
       <c r="L71" s="78"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="78"/>
       <c r="B72" s="78"/>
       <c r="C72" s="78"/>
@@ -2599,7 +2481,7 @@
       <c r="K72" s="78"/>
       <c r="L72" s="78"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="78"/>
       <c r="B73" s="78"/>
       <c r="C73" s="78"/>
@@ -2613,7 +2495,7 @@
       <c r="K73" s="78"/>
       <c r="L73" s="78"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="78"/>
       <c r="B74" s="78"/>
       <c r="C74" s="78"/>
@@ -2627,7 +2509,7 @@
       <c r="K74" s="78"/>
       <c r="L74" s="78"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="78"/>
       <c r="B75" s="78"/>
       <c r="C75" s="78"/>
@@ -2641,7 +2523,7 @@
       <c r="K75" s="78"/>
       <c r="L75" s="78"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="78"/>
       <c r="B76" s="78"/>
       <c r="C76" s="78"/>
@@ -2655,7 +2537,7 @@
       <c r="K76" s="78"/>
       <c r="L76" s="78"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="78"/>
       <c r="B77" s="78"/>
       <c r="C77" s="78"/>
@@ -2669,7 +2551,7 @@
       <c r="K77" s="78"/>
       <c r="L77" s="78"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="78"/>
       <c r="B78" s="78"/>
       <c r="C78" s="78"/>
@@ -13409,22 +13291,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="46">
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="I54:L54"/>
-    <mergeCell ref="A50:L50"/>
-    <mergeCell ref="A51:L51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:L52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:L53"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="C49:E49"/>
+  <mergeCells count="31">
     <mergeCell ref="H36:K36"/>
     <mergeCell ref="D38:D44"/>
     <mergeCell ref="C38:C44"/>
@@ -13457,7 +13324,7 @@
     <mergeCell ref="C15:L15"/>
     <mergeCell ref="C16:L16"/>
   </mergeCells>
-  <pageMargins left="0.31496062992126" right="0.31496062992126" top="0" bottom="0.23622047244093999" header="0.11811023622047" footer="0.11811023622047"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0" bottom="0.23622047244094491" header="0.11811023622047245" footer="0.11811023622047245"/>
   <pageSetup paperSize="9" scale="87" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
commit changes on pr, rfq and awarding of supp
</commit_message>
<xml_diff>
--- a/export_rfq.xlsx
+++ b/export_rfq.xlsx
@@ -1,29 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\fas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72501F07-7C63-4FDE-862A-64F409B1A192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="RFQ Sample" sheetId="1" r:id="rId1"/>
+    <sheet name="RFQ Sample" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'RFQ Sample'!$A$1:$J$103</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>Republic of the Philippines</t>
   </si>
@@ -37,13 +31,13 @@
     <t xml:space="preserve">MODE OF PROCUREMENT: </t>
   </si>
   <si>
-    <t>Small Value Procurement</t>
+    <t>Shopping</t>
   </si>
   <si>
     <t>RFQ No. :</t>
   </si>
   <si>
-    <t>2021-0210</t>
+    <t>2022-00002</t>
   </si>
   <si>
     <t>Name of Procuring Entity:</t>
@@ -55,13 +49,13 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>September 21, 2021</t>
+    <t>March 17, 2022</t>
   </si>
   <si>
     <t>Office/End User:</t>
   </si>
   <si>
-    <t>FAD</t>
+    <t>ORD</t>
   </si>
   <si>
     <t>Company Name:</t>
@@ -112,7 +106,7 @@
     <t>APPROVED BUDGET FOR THE CONTRACT (ABC):</t>
   </si>
   <si>
-    <t>PHP 537,800.00</t>
+    <t>PHP 2,260.00</t>
   </si>
   <si>
     <t>DR. CARINA S. CRUZ</t>
@@ -139,22 +133,25 @@
     <t>PRICE PER UNIT</t>
   </si>
   <si>
-    <t>Warranty</t>
-  </si>
-  <si>
-    <t>Price Validity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                         After having carefully read and accepted your General Conditions, I/WE quote on the item(s) at prices noted above.</t>
-  </si>
-  <si>
-    <t>Printed Name/Signature/Date</t>
-  </si>
-  <si>
-    <t>Revised Form 2012</t>
-  </si>
-  <si>
-    <t>Tel. No./Cellphone No.</t>
+    <t>Clinical Foot Pedal Bin
+TEST 3</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>2,000.00</t>
+  </si>
+  <si>
+    <t>Disposable Isolation Gown
+TEST 3</t>
+  </si>
+  <si>
+    <t>Medical Cap
+TEST 3</t>
+  </si>
+  <si>
+    <t>pack</t>
   </si>
   <si>
     <t>NOTE:
@@ -171,89 +168,143 @@
        a. Email us at dilg4a.bac@gmail.com
        b. Deliver on hand at the receiving area of DILG IV-A CALABARZON, Andenson Bldg1. National Highway, Parian, Calamba City, Laguna</t>
   </si>
+  <si>
+    <t>Warranty</t>
+  </si>
+  <si>
+    <t>Price Validity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                         After having carefully read and accepted your General Conditions, I/WE quote on the item(s) at prices noted above.</t>
+  </si>
+  <si>
+    <t>Printed Name/Signature/Date</t>
+  </si>
+  <si>
+    <t>Revised Form 2012</t>
+  </si>
+  <si>
+    <t>Tel. No./Cellphone No.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="[$PHP]\ #,##0.00;[Red][$PHP]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="[$PHP]\ #,##0.00;[Red][$PHP]\ #,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -261,177 +312,137 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="18">
+    <border/>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -440,550 +451,457 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+  <cellXfs count="139">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="2" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="165" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="3" fillId="2" borderId="9" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" quotePrefix="1" numFmtId="3" fillId="2" borderId="9" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="3" fillId="2" borderId="9" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="3" fillId="2" borderId="10" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" quotePrefix="1" numFmtId="3" fillId="2" borderId="8" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="3" fillId="2" borderId="10" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="3" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" quotePrefix="1" numFmtId="3" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="3" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="3" fillId="2" borderId="8" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="3" fillId="2" borderId="10" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" quotePrefix="1" numFmtId="3" fillId="2" borderId="9" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="3" fillId="2" borderId="9" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="9" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="9" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="9" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" quotePrefix="1" numFmtId="166" fillId="2" borderId="7" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="166" fillId="2" borderId="8" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="17" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="11" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="11" numFmtId="167" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="11" numFmtId="167" fillId="2" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="11" numFmtId="167" fillId="2" borderId="6" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="11" numFmtId="167" fillId="2" borderId="7" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="11" numFmtId="167" fillId="2" borderId="8" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="9" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="9" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -999,13 +917,7 @@
     <xdr:ext cx="552450" cy="533400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 36">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="1" name="Picture 36" descr=""/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1017,10 +929,7 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
+        <a:xfrm rot="0"/>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1074,7 +983,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1107,26 +1016,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1159,23 +1051,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1351,37 +1226,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P103"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:J9"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="130" zoomScaleNormal="130" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.88671875" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="true" style="1"/>
     <col min="2" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="6.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" customWidth="true" style="1"/>
     <col min="4" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="true" style="1"/>
+    <col min="6" max="6" width="14" customWidth="true" style="1"/>
+    <col min="7" max="7" width="8" customWidth="true" style="1"/>
+    <col min="8" max="8" width="9.109375" customWidth="true" style="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="true" style="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="true" style="1"/>
     <col min="11" max="11" width="8.88671875" style="1"/>
-    <col min="12" max="12" width="11.5546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" style="1" customWidth="1"/>
-    <col min="14" max="15" width="11.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="true" style="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="true" style="1"/>
+    <col min="14" max="14" width="11.5546875" customWidth="true" style="1"/>
+    <col min="15" max="15" width="11.5546875" customWidth="true" style="1"/>
     <col min="16" max="16" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +1272,7 @@
       <c r="I1" s="101"/>
       <c r="J1" s="102"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" s="103" t="s">
         <v>1</v>
       </c>
@@ -1409,7 +1286,7 @@
       <c r="I2" s="104"/>
       <c r="J2" s="105"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" s="106" t="s">
         <v>2</v>
       </c>
@@ -1423,7 +1300,7 @@
       <c r="I3" s="107"/>
       <c r="J3" s="108"/>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" customHeight="1" ht="15">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1435,7 +1312,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" customHeight="1" ht="16.5">
       <c r="A5" s="109" t="s">
         <v>3</v>
       </c>
@@ -1455,7 +1332,7 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="A6" s="64" t="s">
         <v>7</v>
       </c>
@@ -1475,7 +1352,7 @@
       </c>
       <c r="J6" s="79"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7" s="64" t="s">
         <v>11</v>
       </c>
@@ -1491,7 +1368,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="A8" s="64" t="s">
         <v>13</v>
       </c>
@@ -1505,7 +1382,7 @@
       <c r="I8" s="66"/>
       <c r="J8" s="67"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="A9" s="64" t="s">
         <v>14</v>
       </c>
@@ -1519,7 +1396,7 @@
       <c r="I9" s="83"/>
       <c r="J9" s="84"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" customHeight="1" ht="15.75">
       <c r="A10" s="85" t="s">
         <v>15</v>
       </c>
@@ -1535,7 +1412,7 @@
       <c r="I10" s="66"/>
       <c r="J10" s="67"/>
     </row>
-    <row r="11" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" customHeight="1" ht="14.4">
       <c r="A11" s="68" t="s">
         <v>17</v>
       </c>
@@ -1549,7 +1426,7 @@
       <c r="I11" s="69"/>
       <c r="J11" s="70"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" s="71"/>
       <c r="B12" s="72"/>
       <c r="C12" s="72"/>
@@ -1561,7 +1438,7 @@
       <c r="I12" s="72"/>
       <c r="J12" s="73"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16">
       <c r="A13" s="74" t="s">
         <v>18</v>
       </c>
@@ -1575,7 +1452,7 @@
       <c r="I13" s="76"/>
       <c r="J13" s="77"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="A14" s="87" t="s">
         <v>19</v>
       </c>
@@ -1591,7 +1468,7 @@
       <c r="I14" s="88"/>
       <c r="J14" s="89"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="A15" s="90"/>
       <c r="B15" s="91"/>
       <c r="C15" s="91"/>
@@ -1603,7 +1480,7 @@
       <c r="I15" s="91"/>
       <c r="J15" s="92"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16">
       <c r="A16" s="93" t="s">
         <v>21</v>
       </c>
@@ -1619,7 +1496,7 @@
       <c r="I16" s="91"/>
       <c r="J16" s="92"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16">
       <c r="A17" s="90" t="s">
         <v>23</v>
       </c>
@@ -1633,7 +1510,7 @@
       <c r="I17" s="91"/>
       <c r="J17" s="92"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16">
       <c r="A18" s="90"/>
       <c r="B18" s="91"/>
       <c r="C18" s="91"/>
@@ -1647,7 +1524,7 @@
       <c r="I18" s="91"/>
       <c r="J18" s="92"/>
     </row>
-    <row r="19" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" customHeight="1" ht="13.95">
       <c r="A19" s="90" t="s">
         <v>25</v>
       </c>
@@ -1661,7 +1538,7 @@
       <c r="I19" s="91"/>
       <c r="J19" s="92"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16">
       <c r="A20" s="90"/>
       <c r="B20" s="91"/>
       <c r="C20" s="91"/>
@@ -1673,7 +1550,7 @@
       <c r="I20" s="91"/>
       <c r="J20" s="92"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16">
       <c r="A21" s="90" t="s">
         <v>26</v>
       </c>
@@ -1687,7 +1564,7 @@
       <c r="I21" s="91"/>
       <c r="J21" s="92"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16">
       <c r="A22" s="90"/>
       <c r="B22" s="91"/>
       <c r="C22" s="91"/>
@@ -1699,7 +1576,7 @@
       <c r="I22" s="91"/>
       <c r="J22" s="92"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16">
       <c r="A23" s="90" t="s">
         <v>27</v>
       </c>
@@ -1713,7 +1590,7 @@
       <c r="I23" s="20"/>
       <c r="J23" s="21"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16">
       <c r="A24" s="90"/>
       <c r="B24" s="91"/>
       <c r="C24" s="91"/>
@@ -1725,7 +1602,7 @@
       <c r="I24" s="20"/>
       <c r="J24" s="21"/>
     </row>
-    <row r="25" spans="1:16" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" customHeight="1" ht="21.6">
       <c r="A25" s="115"/>
       <c r="B25" s="116"/>
       <c r="C25" s="116"/>
@@ -1738,7 +1615,7 @@
       <c r="J25" s="18"/>
       <c r="M25" s="9"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16">
       <c r="A26" s="118" t="s">
         <v>28</v>
       </c>
@@ -1753,7 +1630,7 @@
       <c r="J26" s="12"/>
       <c r="M26" s="9"/>
     </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" customHeight="1" ht="15.75">
       <c r="A27" s="121" t="s">
         <v>29</v>
       </c>
@@ -1770,7 +1647,7 @@
       <c r="J27" s="129"/>
       <c r="M27" s="9"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16">
       <c r="A28" s="124"/>
       <c r="B28" s="125"/>
       <c r="C28" s="125"/>
@@ -1784,7 +1661,7 @@
       <c r="I28" s="131"/>
       <c r="J28" s="132"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16">
       <c r="A29" s="96" t="s">
         <v>32</v>
       </c>
@@ -1809,7 +1686,7 @@
       </c>
       <c r="M29" s="9"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16">
       <c r="A30" s="97"/>
       <c r="B30" s="103"/>
       <c r="C30" s="104"/>
@@ -1821,16 +1698,26 @@
       <c r="I30" s="134"/>
       <c r="J30" s="82"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="39"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
+    <row r="31" spans="1:16">
+      <c r="A31" s="136">
+        <v>1</v>
+      </c>
+      <c r="B31" s="138" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="137"/>
+      <c r="D31" s="137"/>
+      <c r="E31" s="137"/>
       <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
+      <c r="G31" s="40">
+        <v>1</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="135" t="s">
+        <v>40</v>
+      </c>
       <c r="J31" s="39"/>
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
@@ -1839,16 +1726,26 @@
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="39"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
+    <row r="32" spans="1:16">
+      <c r="A32" s="136">
+        <v>2</v>
+      </c>
+      <c r="B32" s="138" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="137"/>
+      <c r="D32" s="137"/>
+      <c r="E32" s="137"/>
       <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
+      <c r="G32" s="40">
+        <v>1</v>
+      </c>
+      <c r="H32" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" s="135">
+        <v>80</v>
+      </c>
       <c r="J32" s="39"/>
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
@@ -1857,16 +1754,26 @@
       <c r="O32" s="24"/>
       <c r="P32" s="24"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A33" s="39"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
+    <row r="33" spans="1:16">
+      <c r="A33" s="136">
+        <v>3</v>
+      </c>
+      <c r="B33" s="138" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="137"/>
+      <c r="D33" s="137"/>
+      <c r="E33" s="137"/>
       <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
+      <c r="G33" s="40">
+        <v>1</v>
+      </c>
+      <c r="H33" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="135">
+        <v>180</v>
+      </c>
       <c r="J33" s="39"/>
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
@@ -1875,7 +1782,7 @@
       <c r="O33" s="24"/>
       <c r="P33" s="24"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" customHeight="1" ht="250">
       <c r="A34" s="39"/>
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
@@ -1893,7 +1800,7 @@
       <c r="O34" s="24"/>
       <c r="P34" s="24"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16">
       <c r="A35" s="39"/>
       <c r="B35" s="40"/>
       <c r="C35" s="40"/>
@@ -1911,7 +1818,7 @@
       <c r="O35" s="24"/>
       <c r="P35" s="24"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16">
       <c r="A36" s="39"/>
       <c r="B36" s="40"/>
       <c r="C36" s="40"/>
@@ -1929,7 +1836,7 @@
       <c r="O36" s="24"/>
       <c r="P36" s="24"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16">
       <c r="A37" s="39"/>
       <c r="B37" s="40"/>
       <c r="C37" s="40"/>
@@ -1947,7 +1854,7 @@
       <c r="O37" s="24"/>
       <c r="P37" s="24"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16">
       <c r="A38" s="39"/>
       <c r="B38" s="40"/>
       <c r="C38" s="40"/>
@@ -1965,7 +1872,7 @@
       <c r="O38" s="24"/>
       <c r="P38" s="24"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16">
       <c r="A39" s="39"/>
       <c r="B39" s="40"/>
       <c r="C39" s="40"/>
@@ -1983,7 +1890,7 @@
       <c r="O39" s="24"/>
       <c r="P39" s="24"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16">
       <c r="A40" s="39"/>
       <c r="B40" s="40"/>
       <c r="C40" s="40"/>
@@ -2001,7 +1908,7 @@
       <c r="O40" s="24"/>
       <c r="P40" s="24"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16">
       <c r="A41" s="39"/>
       <c r="B41" s="40"/>
       <c r="C41" s="40"/>
@@ -2019,7 +1926,7 @@
       <c r="O41" s="24"/>
       <c r="P41" s="24"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16">
       <c r="A42" s="39"/>
       <c r="B42" s="40"/>
       <c r="C42" s="40"/>
@@ -2037,7 +1944,7 @@
       <c r="O42" s="24"/>
       <c r="P42" s="24"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16">
       <c r="A43" s="39"/>
       <c r="B43" s="40"/>
       <c r="C43" s="40"/>
@@ -2055,7 +1962,7 @@
       <c r="O43" s="24"/>
       <c r="P43" s="24"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16">
       <c r="A44" s="39"/>
       <c r="B44" s="40"/>
       <c r="C44" s="40"/>
@@ -2073,7 +1980,7 @@
       <c r="O44" s="24"/>
       <c r="P44" s="24"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16">
       <c r="A45" s="39"/>
       <c r="B45" s="40"/>
       <c r="C45" s="40"/>
@@ -2091,7 +1998,7 @@
       <c r="O45" s="24"/>
       <c r="P45" s="24"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16">
       <c r="A46" s="39"/>
       <c r="B46" s="40"/>
       <c r="C46" s="40"/>
@@ -2109,7 +2016,7 @@
       <c r="O46" s="24"/>
       <c r="P46" s="24"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16">
       <c r="A47" s="39"/>
       <c r="B47" s="40"/>
       <c r="C47" s="40"/>
@@ -2127,7 +2034,7 @@
       <c r="O47" s="24"/>
       <c r="P47" s="24"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16">
       <c r="A48" s="39"/>
       <c r="B48" s="40"/>
       <c r="C48" s="40"/>
@@ -2145,7 +2052,7 @@
       <c r="O48" s="24"/>
       <c r="P48" s="24"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16">
       <c r="A49" s="39"/>
       <c r="B49" s="40"/>
       <c r="C49" s="40"/>
@@ -2163,7 +2070,7 @@
       <c r="O49" s="24"/>
       <c r="P49" s="24"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16">
       <c r="A50" s="39"/>
       <c r="B50" s="40"/>
       <c r="C50" s="40"/>
@@ -2181,7 +2088,7 @@
       <c r="O50" s="24"/>
       <c r="P50" s="24"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16">
       <c r="A51" s="39"/>
       <c r="B51" s="40"/>
       <c r="C51" s="40"/>
@@ -2199,7 +2106,7 @@
       <c r="O51" s="24"/>
       <c r="P51" s="24"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16">
       <c r="A52" s="39"/>
       <c r="B52" s="40"/>
       <c r="C52" s="40"/>
@@ -2217,7 +2124,7 @@
       <c r="O52" s="24"/>
       <c r="P52" s="24"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16">
       <c r="A53" s="39"/>
       <c r="B53" s="40"/>
       <c r="C53" s="40"/>
@@ -2235,7 +2142,7 @@
       <c r="O53" s="24"/>
       <c r="P53" s="24"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16">
       <c r="A54" s="39"/>
       <c r="B54" s="40"/>
       <c r="C54" s="40"/>
@@ -2253,7 +2160,7 @@
       <c r="O54" s="24"/>
       <c r="P54" s="24"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16">
       <c r="A55" s="39"/>
       <c r="B55" s="40"/>
       <c r="C55" s="40"/>
@@ -2271,7 +2178,7 @@
       <c r="O55" s="24"/>
       <c r="P55" s="24"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16">
       <c r="A56" s="39"/>
       <c r="B56" s="40"/>
       <c r="C56" s="40"/>
@@ -2289,7 +2196,7 @@
       <c r="O56" s="24"/>
       <c r="P56" s="24"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16">
       <c r="A57" s="39"/>
       <c r="B57" s="40"/>
       <c r="C57" s="40"/>
@@ -2307,7 +2214,7 @@
       <c r="O57" s="24"/>
       <c r="P57" s="24"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16">
       <c r="A58" s="39"/>
       <c r="B58" s="40"/>
       <c r="C58" s="40"/>
@@ -2325,7 +2232,7 @@
       <c r="O58" s="24"/>
       <c r="P58" s="24"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16">
       <c r="A59" s="39"/>
       <c r="B59" s="40"/>
       <c r="C59" s="40"/>
@@ -2343,7 +2250,7 @@
       <c r="O59" s="24"/>
       <c r="P59" s="24"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16">
       <c r="A60" s="39"/>
       <c r="B60" s="40"/>
       <c r="C60" s="40"/>
@@ -2361,7 +2268,7 @@
       <c r="O60" s="24"/>
       <c r="P60" s="24"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16">
       <c r="A61" s="39"/>
       <c r="B61" s="40"/>
       <c r="C61" s="40"/>
@@ -2379,7 +2286,7 @@
       <c r="O61" s="24"/>
       <c r="P61" s="24"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16">
       <c r="A62" s="39"/>
       <c r="B62" s="40"/>
       <c r="C62" s="40"/>
@@ -2397,7 +2304,7 @@
       <c r="O62" s="24"/>
       <c r="P62" s="24"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16">
       <c r="A63" s="39"/>
       <c r="B63" s="40"/>
       <c r="C63" s="40"/>
@@ -2415,7 +2322,7 @@
       <c r="O63" s="24"/>
       <c r="P63" s="24"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16">
       <c r="A64" s="39"/>
       <c r="B64" s="40"/>
       <c r="C64" s="40"/>
@@ -2433,7 +2340,7 @@
       <c r="O64" s="24"/>
       <c r="P64" s="24"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16">
       <c r="A65" s="39"/>
       <c r="B65" s="40"/>
       <c r="C65" s="40"/>
@@ -2451,7 +2358,7 @@
       <c r="O65" s="24"/>
       <c r="P65" s="24"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16">
       <c r="A66" s="39"/>
       <c r="B66" s="40"/>
       <c r="C66" s="40"/>
@@ -2469,7 +2376,7 @@
       <c r="O66" s="24"/>
       <c r="P66" s="24"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16">
       <c r="A67" s="39"/>
       <c r="B67" s="40"/>
       <c r="C67" s="40"/>
@@ -2487,7 +2394,7 @@
       <c r="O67" s="24"/>
       <c r="P67" s="24"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16">
       <c r="A68" s="39"/>
       <c r="B68" s="40"/>
       <c r="C68" s="40"/>
@@ -2505,7 +2412,7 @@
       <c r="O68" s="24"/>
       <c r="P68" s="24"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16">
       <c r="A69" s="39"/>
       <c r="B69" s="40"/>
       <c r="C69" s="40"/>
@@ -2523,7 +2430,7 @@
       <c r="O69" s="24"/>
       <c r="P69" s="24"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16">
       <c r="A70" s="39"/>
       <c r="B70" s="40"/>
       <c r="C70" s="40"/>
@@ -2541,7 +2448,7 @@
       <c r="O70" s="24"/>
       <c r="P70" s="24"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16">
       <c r="A71" s="39"/>
       <c r="B71" s="40"/>
       <c r="C71" s="40"/>
@@ -2559,7 +2466,7 @@
       <c r="O71" s="24"/>
       <c r="P71" s="24"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16">
       <c r="A72" s="39"/>
       <c r="B72" s="40"/>
       <c r="C72" s="40"/>
@@ -2577,7 +2484,7 @@
       <c r="O72" s="24"/>
       <c r="P72" s="24"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16">
       <c r="A73" s="39"/>
       <c r="B73" s="40"/>
       <c r="C73" s="40"/>
@@ -2595,7 +2502,7 @@
       <c r="O73" s="24"/>
       <c r="P73" s="24"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16">
       <c r="A74" s="39"/>
       <c r="B74" s="40"/>
       <c r="C74" s="40"/>
@@ -2613,7 +2520,7 @@
       <c r="O74" s="24"/>
       <c r="P74" s="24"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16">
       <c r="A75" s="39"/>
       <c r="B75" s="40"/>
       <c r="C75" s="40"/>
@@ -2631,7 +2538,7 @@
       <c r="O75" s="24"/>
       <c r="P75" s="24"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16">
       <c r="A76" s="39"/>
       <c r="B76" s="40"/>
       <c r="C76" s="40"/>
@@ -2649,7 +2556,7 @@
       <c r="O76" s="24"/>
       <c r="P76" s="24"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16">
       <c r="A77" s="39"/>
       <c r="B77" s="40"/>
       <c r="C77" s="40"/>
@@ -2667,7 +2574,7 @@
       <c r="O77" s="24"/>
       <c r="P77" s="24"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16">
       <c r="A78" s="39"/>
       <c r="B78" s="40"/>
       <c r="C78" s="40"/>
@@ -2685,7 +2592,7 @@
       <c r="O78" s="24"/>
       <c r="P78" s="24"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16">
       <c r="A79" s="39"/>
       <c r="B79" s="40"/>
       <c r="C79" s="40"/>
@@ -2703,7 +2610,7 @@
       <c r="O79" s="24"/>
       <c r="P79" s="24"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16">
       <c r="A80" s="39"/>
       <c r="B80" s="40"/>
       <c r="C80" s="40"/>
@@ -2721,7 +2628,7 @@
       <c r="O80" s="24"/>
       <c r="P80" s="24"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16">
       <c r="A81" s="39"/>
       <c r="B81" s="40"/>
       <c r="C81" s="40"/>
@@ -2739,7 +2646,7 @@
       <c r="O81" s="24"/>
       <c r="P81" s="24"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16">
       <c r="A82" s="39"/>
       <c r="B82" s="40"/>
       <c r="C82" s="40"/>
@@ -2757,7 +2664,7 @@
       <c r="O82" s="24"/>
       <c r="P82" s="24"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16">
       <c r="A83" s="39"/>
       <c r="B83" s="40"/>
       <c r="C83" s="40"/>
@@ -2775,7 +2682,7 @@
       <c r="O83" s="24"/>
       <c r="P83" s="24"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16">
       <c r="A84" s="39"/>
       <c r="B84" s="40"/>
       <c r="C84" s="40"/>
@@ -2793,7 +2700,7 @@
       <c r="O84" s="24"/>
       <c r="P84" s="24"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16">
       <c r="A85" s="39"/>
       <c r="B85" s="40"/>
       <c r="C85" s="40"/>
@@ -2811,7 +2718,7 @@
       <c r="O85" s="24"/>
       <c r="P85" s="24"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16">
       <c r="A86" s="39"/>
       <c r="B86" s="40"/>
       <c r="C86" s="40"/>
@@ -2829,7 +2736,7 @@
       <c r="O86" s="24"/>
       <c r="P86" s="24"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16">
       <c r="A87" s="39"/>
       <c r="B87" s="40"/>
       <c r="C87" s="40"/>
@@ -2847,7 +2754,7 @@
       <c r="O87" s="24"/>
       <c r="P87" s="24"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16">
       <c r="A88" s="39"/>
       <c r="B88" s="40"/>
       <c r="C88" s="40"/>
@@ -2865,7 +2772,7 @@
       <c r="O88" s="24"/>
       <c r="P88" s="24"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16">
       <c r="A89" s="39"/>
       <c r="B89" s="40"/>
       <c r="C89" s="40"/>
@@ -2883,7 +2790,7 @@
       <c r="O89" s="24"/>
       <c r="P89" s="24"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16">
       <c r="A90" s="39"/>
       <c r="B90" s="40"/>
       <c r="C90" s="40"/>
@@ -2901,7 +2808,7 @@
       <c r="O90" s="24"/>
       <c r="P90" s="24"/>
     </row>
-    <row r="91" spans="1:16" s="13" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" customHeight="1" ht="20.1" s="13" customFormat="1">
       <c r="A91" s="41"/>
       <c r="B91" s="31"/>
       <c r="C91" s="31"/>
@@ -2916,7 +2823,7 @@
       <c r="L91" s="23"/>
       <c r="M91" s="14"/>
     </row>
-    <row r="92" spans="1:16" s="13" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" customHeight="1" ht="20.1" s="13" customFormat="1">
       <c r="A92" s="41"/>
       <c r="B92" s="31"/>
       <c r="C92" s="31"/>
@@ -2931,7 +2838,7 @@
       <c r="L92" s="23"/>
       <c r="M92" s="14"/>
     </row>
-    <row r="93" spans="1:16" s="13" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" customHeight="1" ht="20.1" s="13" customFormat="1">
       <c r="A93" s="42"/>
       <c r="B93" s="31"/>
       <c r="C93" s="31"/>
@@ -2946,7 +2853,7 @@
       <c r="L93" s="23"/>
       <c r="M93" s="14"/>
     </row>
-    <row r="94" spans="1:16" s="13" customFormat="1" ht="349.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" customHeight="1" ht="349.5" s="13" customFormat="1">
       <c r="A94" s="41"/>
       <c r="B94" s="98" t="s">
         <v>44</v>
@@ -2963,7 +2870,7 @@
       <c r="L94" s="23"/>
       <c r="M94" s="14"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16">
       <c r="A95" s="44"/>
       <c r="B95" s="44"/>
       <c r="C95" s="45"/>
@@ -2981,16 +2888,16 @@
       <c r="O95" s="24"/>
       <c r="P95" s="24"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16">
       <c r="A96" s="52" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B96" s="53"/>
       <c r="C96" s="53"/>
       <c r="D96" s="54"/>
       <c r="E96" s="26"/>
       <c r="F96" s="57" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G96" s="58"/>
       <c r="H96" s="55"/>
@@ -3003,7 +2910,7 @@
       <c r="O96" s="24"/>
       <c r="P96" s="24"/>
     </row>
-    <row r="97" spans="1:16" s="15" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" customHeight="1" ht="14.4" s="15" customFormat="1">
       <c r="A97" s="25"/>
       <c r="B97" s="26"/>
       <c r="C97" s="26"/>
@@ -3015,9 +2922,9 @@
       <c r="I97" s="11"/>
       <c r="J97" s="12"/>
     </row>
-    <row r="98" spans="1:16" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" customHeight="1" ht="12.75" s="15" customFormat="1">
       <c r="A98" s="59" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B98" s="60"/>
       <c r="C98" s="60"/>
@@ -3029,7 +2936,7 @@
       <c r="I98" s="60"/>
       <c r="J98" s="61"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16">
       <c r="A99" s="59"/>
       <c r="B99" s="60"/>
       <c r="C99" s="60"/>
@@ -3047,7 +2954,7 @@
       <c r="O99" s="24"/>
       <c r="P99" s="24"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16">
       <c r="A100" s="25"/>
       <c r="B100" s="26"/>
       <c r="C100" s="26"/>
@@ -3065,7 +2972,7 @@
       <c r="O100" s="24"/>
       <c r="P100" s="24"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16">
       <c r="A101" s="25"/>
       <c r="B101" s="26"/>
       <c r="C101" s="26"/>
@@ -3073,7 +2980,7 @@
       <c r="E101" s="26"/>
       <c r="F101" s="26"/>
       <c r="G101" s="62" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H101" s="62"/>
       <c r="I101" s="62"/>
@@ -3085,7 +2992,7 @@
       <c r="O101" s="24"/>
       <c r="P101" s="24"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16">
       <c r="A102" s="25"/>
       <c r="B102" s="26"/>
       <c r="C102" s="26"/>
@@ -3103,9 +3010,9 @@
       <c r="O102" s="24"/>
       <c r="P102" s="24"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16">
       <c r="A103" s="28" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B103" s="29"/>
       <c r="C103" s="29"/>
@@ -3113,15 +3020,15 @@
       <c r="E103" s="29"/>
       <c r="F103" s="29"/>
       <c r="G103" s="63" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H103" s="63"/>
       <c r="I103" s="63"/>
       <c r="J103" s="30"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="45">
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
     <mergeCell ref="I29:I30"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="B94:F94"/>
@@ -3167,9 +3074,21 @@
     <mergeCell ref="E10:J10"/>
     <mergeCell ref="A14:E15"/>
     <mergeCell ref="F14:J15"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
   </mergeCells>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.59055118110236227" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.23622047244094" right="0.23622047244094" top="0.59055118110236" bottom="0.39370078740157" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="97" fitToHeight="0" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>